<commit_message>
Changes to Risk and Index file for Website
</commit_message>
<xml_diff>
--- a/PROJECT FILES/Project Management/RiskManagement_v2.xlsx
+++ b/PROJECT FILES/Project Management/RiskManagement_v2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="90">
   <si>
     <t>Risk #</t>
   </si>
@@ -226,13 +226,73 @@
   </si>
   <si>
     <t>Perform several tests to increase robustness. Have a trained team member solve the technical tasks.</t>
+  </si>
+  <si>
+    <t>Robot does not recognize e-stop command and keeps on moving/damaging the environment.</t>
+  </si>
+  <si>
+    <t>Integrate a hardware e-stop with the robot to control power to the drive system (ie locomotion).</t>
+  </si>
+  <si>
+    <t>Unable to stop during an emergency</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>SOLVED</t>
+  </si>
+  <si>
+    <t>2nd semester</t>
+  </si>
+  <si>
+    <t>Undergoing…</t>
+  </si>
+  <si>
+    <t>Traces of PCB board tear off</t>
+  </si>
+  <si>
+    <t>Technical, Cost</t>
+  </si>
+  <si>
+    <t>PCB traces are too thin to conduct the 6.6A of the on-board electronics at the testing temperature. The traces are likely to tear off the PCB board rendering the on-board electronics useless.</t>
+  </si>
+  <si>
+    <t>(Short-term): Use the 12VDC battery to power the pump separetely from the on-board electronics. (Long-term): make a new PCB board with bigger ground traces.</t>
+  </si>
+  <si>
+    <t>SOLVED (short term)</t>
+  </si>
+  <si>
+    <t>Runs out of paint</t>
+  </si>
+  <si>
+    <t>Robot takes longer than expected and ends up consuming more resources than expected to paint the field. Robot will then require a refill of resources.</t>
+  </si>
+  <si>
+    <t>Calculate the paint consumption rate (0.3038 gal/min). Use the consumption rate and assign an average speed to compute the entire length of time needed to paint a soccer field. Ensure that the robot can hold the entire "predicted" volume of paint to be consumed and a little extra (20% more).</t>
+  </si>
+  <si>
+    <t>Motor controller USB connection breaks loose again</t>
+  </si>
+  <si>
+    <t>The USB comm port of the RoboteQ loses connection and breaks loose again. The computer is then unable to send control commands to the robot making the robot require an e-stop or abort.</t>
+  </si>
+  <si>
+    <t>MFR6, MNFR7</t>
+  </si>
+  <si>
+    <t>MFR1</t>
+  </si>
+  <si>
+    <t>MFR1, MNFR6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,6 +306,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -269,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -287,20 +354,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -315,6 +374,18 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -345,17 +416,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:H15" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A1:H15"/>
-  <tableColumns count="8">
-    <tableColumn id="1" name="Risk #" dataDxfId="0"/>
-    <tableColumn id="2" name="Risk" dataDxfId="1"/>
-    <tableColumn id="3" name="Reqt." dataDxfId="2"/>
-    <tableColumn id="4" name="Type" dataDxfId="3"/>
-    <tableColumn id="5" name="Description" dataDxfId="7"/>
-    <tableColumn id="6" name="Likelihood" dataDxfId="6"/>
-    <tableColumn id="7" name="Consequence" dataDxfId="5"/>
-    <tableColumn id="8" name="Risk Reduction Plan" dataDxfId="4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:I19" totalsRowShown="0" headerRowDxfId="9">
+  <autoFilter ref="A1:I19"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="Risk #" dataDxfId="8"/>
+    <tableColumn id="2" name="Risk" dataDxfId="7"/>
+    <tableColumn id="3" name="Reqt." dataDxfId="6"/>
+    <tableColumn id="4" name="Type" dataDxfId="5"/>
+    <tableColumn id="5" name="Description" dataDxfId="4"/>
+    <tableColumn id="6" name="Likelihood" dataDxfId="3"/>
+    <tableColumn id="7" name="Consequence" dataDxfId="2"/>
+    <tableColumn id="8" name="Risk Reduction Plan" dataDxfId="1"/>
+    <tableColumn id="9" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -648,10 +720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -664,9 +736,10 @@
     <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="54.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -691,10 +764,13 @@
       <c r="H1" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I1" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -717,10 +793,13 @@
       <c r="H2" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I2" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
-        <v>1.2</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
@@ -743,10 +822,13 @@
       <c r="H3" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I3" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <v>2.1</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
@@ -769,10 +851,13 @@
       <c r="H4" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I4" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
-        <v>2.2000000000000002</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>10</v>
@@ -795,10 +880,13 @@
       <c r="H5" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I5" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>3.1</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>11</v>
@@ -821,10 +909,13 @@
       <c r="H6" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I6" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
-        <v>3.2</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>12</v>
@@ -847,10 +938,13 @@
       <c r="H7" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I7" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>13</v>
@@ -873,10 +967,13 @@
       <c r="H8" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I8" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>36</v>
@@ -899,10 +996,13 @@
       <c r="H9" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I9" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>20</v>
@@ -925,10 +1025,13 @@
       <c r="H10" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I10" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>14</v>
@@ -951,10 +1054,13 @@
       <c r="H11" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I11" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
-        <v>8.1</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>27</v>
@@ -977,10 +1083,13 @@
       <c r="H12" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="I12" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
-        <v>8.1999999999999993</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>59</v>
@@ -1003,10 +1112,13 @@
       <c r="H13" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I13" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
-        <v>8.3000000000000007</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>62</v>
@@ -1029,10 +1141,13 @@
       <c r="H14" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I14" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>66</v>
@@ -1055,6 +1170,121 @@
       <c r="H15" s="2" t="s">
         <v>69</v>
       </c>
+      <c r="I15" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="3">
+        <v>2</v>
+      </c>
+      <c r="G16" s="3">
+        <v>3</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17" s="3">
+        <v>4</v>
+      </c>
+      <c r="G17" s="3">
+        <v>5</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" s="3">
+        <v>2</v>
+      </c>
+      <c r="G18" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F19" s="3">
+        <v>3</v>
+      </c>
+      <c r="G19" s="3">
+        <v>3</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>